<commit_message>
class 8 materials added
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmac\Google Drive\courses\databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB924097-B5F0-45DA-9C4E-7654D5BC49D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CA91FB-5419-4B73-947A-D33B6FEEF58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t>Class number</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>7.3.1.5-8</t>
-  </si>
-  <si>
-    <t>SQL: [join with comma], join, inner join … on, left/right/full outer join, nested queries, correlated queries, all, any</t>
   </si>
   <si>
     <t>SQL: exists, union, intersect, except, insert into … values, delete from, update … set, alter table … add</t>
@@ -378,22 +375,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">mapping ER/EER to relational model
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF002060"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SQL: order by, asc, desc</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">lightly read ch4;
 carefully read 6.1 and </t>
     </r>
@@ -559,6 +540,9 @@
       </rPr>
       <t>(Skip 1NF, 2NF and 4NF. We study only BCNF and 3NF. Use definitions provided in class for these.)</t>
     </r>
+  </si>
+  <si>
+    <t>SQL: [implicit join with comma], join, inner join … on, left/right/full outer join, nested queries, correlated queries, all, any</t>
   </si>
 </sst>
 </file>
@@ -1257,8 +1241,8 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,13 +1276,13 @@
         <v>0</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1320,7 +1304,7 @@
       <c r="F2" s="43"/>
       <c r="G2" s="22"/>
       <c r="H2" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1333,17 +1317,17 @@
         <v>44588</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="43"/>
       <c r="G3" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>89</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1364,13 +1348,13 @@
         <v>8</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="22">
         <v>3.3</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1390,13 +1374,13 @@
         <v>9</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -1418,13 +1402,13 @@
       </c>
       <c r="F6" s="43"/>
       <c r="G6" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="31" t="str">
         <f t="shared" si="1"/>
@@ -1440,10 +1424,12 @@
       </c>
       <c r="F7" s="43"/>
       <c r="G7" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="H7" s="13" t="s">
         <v>92</v>
+      </c>
+      <c r="H7" s="13" t="e">
+        <f>H16
+                                                                                                                                                                                                                                                                SQL: order by, asc, desc</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1466,13 +1452,13 @@
         <v>12</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1494,7 +1480,7 @@
         <v>50</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>51</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1515,13 +1501,13 @@
         <v>14</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H10" s="39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1540,10 +1526,10 @@
       </c>
       <c r="F11" s="43"/>
       <c r="G11" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="40" t="s">
         <v>54</v>
-      </c>
-      <c r="H11" s="40" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1566,7 +1552,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="24"/>
       <c r="H12" s="18"/>
@@ -1612,10 +1598,10 @@
       </c>
       <c r="F14" s="43"/>
       <c r="G14" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1629,13 +1615,13 @@
         <v>44630</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="13"/>
@@ -1693,13 +1679,13 @@
         <v>20</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I18" s="10"/>
     </row>
@@ -1719,13 +1705,13 @@
       </c>
       <c r="F19" s="43"/>
       <c r="G19" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <f>A18+1</f>
         <v>9</v>
@@ -1745,10 +1731,10 @@
         <v>22</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H20" s="13"/>
     </row>
@@ -1763,13 +1749,13 @@
         <v>44651</v>
       </c>
       <c r="D21" s="51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F21" s="46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G21" s="23"/>
       <c r="H21" s="13"/>
@@ -1792,12 +1778,12 @@
         <v>24</v>
       </c>
       <c r="F22" s="46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G22" s="30"/>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="31" t="str">
         <f t="shared" si="1"/>
@@ -1815,10 +1801,10 @@
       </c>
       <c r="F23" s="46"/>
       <c r="G23" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1839,10 +1825,10 @@
         <v>26</v>
       </c>
       <c r="G24" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24" s="13" t="s">
         <v>99</v>
-      </c>
-      <c r="H24" s="13" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1862,10 +1848,10 @@
         <v>27</v>
       </c>
       <c r="F25" s="43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G25" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H25" s="13"/>
     </row>
@@ -1889,7 +1875,7 @@
         <v>28</v>
       </c>
       <c r="F26" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G26" s="23"/>
       <c r="H26" s="13"/>
@@ -1927,19 +1913,19 @@
         <v>44676</v>
       </c>
       <c r="D28" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F28" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G28" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H28" s="57" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -1978,7 +1964,7 @@
         <v>32</v>
       </c>
       <c r="F30" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G30" s="55"/>
       <c r="H30" s="58"/>
@@ -2014,7 +2000,7 @@
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G32" s="22"/>
       <c r="H32" s="13"/>

</xml_diff>